<commit_message>
#456 Add test case
</commit_message>
<xml_diff>
--- a/src/test/resources/1.xlsx
+++ b/src/test/resources/1.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wangguanquan3\eec\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangguanquan3/eec/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DE7054-5B1E-F742-90F3-00478370F0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="525" windowWidth="18015" windowHeight="10350"/>
+    <workbookView xWindow="17800" yWindow="9820" windowWidth="18020" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object测试" sheetId="1" r:id="rId1"/>
+    <sheet name="header rows test" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Object测试!$A$1:$F$1</definedName>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="131">
   <si>
     <t>极品飞车</t>
   </si>
@@ -412,26 +414,31 @@
   </si>
   <si>
     <t>Ae9CNO6eTu</t>
+  </si>
+  <si>
+    <t>账号</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -444,7 +451,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -496,7 +518,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -506,7 +528,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -518,7 +540,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -526,6 +548,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,9 +582,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -585,9 +622,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -622,7 +659,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -657,7 +694,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -830,7 +867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -838,17 +875,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" customHeight="1">
+    <row r="1" spans="1:6" ht="18.5" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>30</v>
       </c>
@@ -2749,9 +2786,85 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <picture r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C0689A-9935-8144-86F5-C3003FE75A5F}">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="10">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="12">
+        <v>43425</v>
+      </c>
+      <c r="E4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="10">
+        <v>8</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="12">
+        <v>43425</v>
+      </c>
+      <c r="E5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>